<commit_message>
Finished integrating webscraper with classifier.
</commit_message>
<xml_diff>
--- a/website_classifications_bins.xlsx
+++ b/website_classifications_bins.xlsx
@@ -5,27 +5,29 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clj00\Documents\Classes\Computational Intelligence\Assignment1\python-web-scraper\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clj00\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10827" xr2:uid="{D81EADFC-6E95-4979-817D-99A82B9ED314}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10827" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="62">
   <si>
     <t>[-0.5…0.0]</t>
   </si>
@@ -166,13 +168,58 @@
   </si>
   <si>
     <t>https://www.msn.com</t>
+  </si>
+  <si>
+    <t>Prediction (GRNN)</t>
+  </si>
+  <si>
+    <t>Prediction (URLVoid)</t>
+  </si>
+  <si>
+    <t>GRNN Interpretation</t>
+  </si>
+  <si>
+    <t>safe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">malicious </t>
+  </si>
+  <si>
+    <t>malicious</t>
+  </si>
+  <si>
+    <t>no data</t>
+  </si>
+  <si>
+    <t>unsafe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">less than 80 is considered bad </t>
+  </si>
+  <si>
+    <t>Predict(Web of trust )</t>
+  </si>
+  <si>
+    <t>No data</t>
+  </si>
+  <si>
+    <t>http://trinidadbeat.com/doc/dsign/</t>
+  </si>
+  <si>
+    <t>http://tpi110225014zn.xyz/fpx11801147411nz.it</t>
+  </si>
+  <si>
+    <t>http://barcelonabestlodge.com/motor/box/</t>
+  </si>
+  <si>
+    <t>http://gestarse.org/sigin/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -210,15 +257,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -228,6 +268,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -244,17 +296,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -569,349 +628,806 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A1D0756-A75E-4D85-A04B-C921BAF2E252}">
-  <dimension ref="B1:I13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B1:U18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="112" workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="8.8203125" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="11" style="3" customWidth="1"/>
-    <col min="2" max="2" width="56.46875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="10.52734375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="30.703125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="8.9375" style="3"/>
-    <col min="6" max="6" width="52.87890625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="8.9375" style="3"/>
-    <col min="8" max="8" width="91.5859375" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="8.9375" style="3"/>
+    <col min="1" max="1" width="11" style="2" customWidth="1"/>
+    <col min="2" max="2" width="56.46875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="15" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="17" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.46875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.64453125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="8.8203125" style="2"/>
+    <col min="9" max="10" width="17" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.46875" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="52.8203125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="8.8203125" style="2"/>
+    <col min="14" max="15" width="17" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.46875" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="91.64453125" style="2" customWidth="1"/>
+    <col min="18" max="18" width="8.8203125" style="2"/>
+    <col min="19" max="21" width="17" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="8.8203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.5">
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="2:21" x14ac:dyDescent="0.5">
+      <c r="B1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-    </row>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.5">
-      <c r="B2" s="6" t="s">
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+    </row>
+    <row r="2" spans="2:21" x14ac:dyDescent="0.5">
+      <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6" t="s">
+      <c r="C2" s="7"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6" t="s">
+      <c r="H2" s="7"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6" t="s">
+      <c r="M2" s="7"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="6"/>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.5">
-      <c r="B3" s="7" t="s">
+      <c r="R2" s="7"/>
+    </row>
+    <row r="3" spans="2:21" x14ac:dyDescent="0.5">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="I3" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="L3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="M3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="N3" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="R3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.5">
-      <c r="B4" s="5" t="s">
+      <c r="S3" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="T3" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="U3" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="2:21" x14ac:dyDescent="0.5">
+      <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>-0.66666000000000003</v>
       </c>
       <c r="D4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="3">
+      <c r="H4" s="2">
         <v>-0.33333000000000002</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="I4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="L4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="3">
+      <c r="M4" s="2">
         <v>0.33333000000000002</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="N4" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="O4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="3">
+      <c r="R4" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.5">
-      <c r="B5" s="5" t="s">
+      <c r="S4" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="T4" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="U4" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="2:21" x14ac:dyDescent="0.5">
+      <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>-0.66666000000000003</v>
       </c>
       <c r="D5" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="3">
+      <c r="H5" s="2">
         <v>-0.33333000000000002</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="I5" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="L5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="3">
+      <c r="M5" s="2">
         <v>0.33333000000000002</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="N5" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="P5" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q5" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="I5" s="3">
+      <c r="R5" s="2">
         <v>0.66666000000000003</v>
       </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.5">
-      <c r="B6" s="5" t="s">
+      <c r="S5" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="U5" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="2:21" x14ac:dyDescent="0.5">
+      <c r="B6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>-1</v>
       </c>
       <c r="D6" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="3">
+      <c r="H6" s="2">
         <v>-0.33333000000000002</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="I6" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="L6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="3">
+      <c r="M6" s="2">
         <v>0.33333000000000002</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="N6" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="O6" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="P6" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q6" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="R6" s="2">
+        <v>0.66666000000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="2:21" x14ac:dyDescent="0.5">
+      <c r="B7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="2">
+        <v>-0.33333000000000002</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M7" s="2">
+        <v>0.33333000000000002</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="O7" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="P7" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q7" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="R7" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:21" x14ac:dyDescent="0.5">
+      <c r="B8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="2">
+        <v>-0.66666000000000003</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" s="2">
+        <v>-0.33333000000000002</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="M8" s="2">
+        <v>0.33333000000000002</v>
+      </c>
+      <c r="N8" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="O8" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="P8" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R8" s="2">
+        <v>0.66666000000000003</v>
+      </c>
+      <c r="S8" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="T8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="U8" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="2:21" x14ac:dyDescent="0.5">
+      <c r="B9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="2">
+        <v>-0.66666000000000003</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" s="2">
+        <v>-0.33333000000000002</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="M9" s="2">
+        <v>0</v>
+      </c>
+      <c r="N9" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="O9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="P9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R9" s="2">
+        <v>0.66666000000000003</v>
+      </c>
+      <c r="S9" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="T9" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="U9" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="2:21" x14ac:dyDescent="0.5">
+      <c r="B10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" s="2">
+        <v>-0.33333000000000002</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="M10" s="2">
+        <v>0</v>
+      </c>
+      <c r="N10" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="O10" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="P10" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="R10" s="2">
+        <v>1</v>
+      </c>
+      <c r="S10" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="T10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="U10" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="2:21" x14ac:dyDescent="0.5">
+      <c r="B11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="2">
+        <v>-0.66666000000000003</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H11" s="2">
+        <v>-0.33333000000000002</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="L11" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="M11" s="2">
+        <v>0</v>
+      </c>
+      <c r="N11" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="O11" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="P11" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q11" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="R11" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:21" x14ac:dyDescent="0.5">
+      <c r="B12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H12" s="2">
+        <v>-0.33333000000000002</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M12" s="2">
+        <v>0</v>
+      </c>
+      <c r="N12" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="O12" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="P12" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="R12" s="2">
+        <v>0.66666000000000003</v>
+      </c>
+      <c r="S12" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="T12" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="U12" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="2:21" x14ac:dyDescent="0.5">
+      <c r="B13" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="2">
+        <v>-0.66666000000000003</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H13" s="2">
+        <v>-0.33333000000000002</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M13" s="2">
+        <v>0.33333000000000002</v>
+      </c>
+      <c r="N13" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="O13" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="P13" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q13" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="R13" s="5">
+        <v>0.66666000000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="2:21" x14ac:dyDescent="0.5">
+      <c r="Q15" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="I6" s="3">
+      <c r="R15" s="10">
         <v>0.66666000000000003</v>
       </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.5">
-      <c r="B7" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="3">
-        <v>-1</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="3">
-        <v>-0.33333000000000002</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" s="3">
-        <v>0.33333000000000002</v>
-      </c>
-      <c r="H7" s="1" t="s">
+      <c r="S15" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="T15" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="U15" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="2:21" x14ac:dyDescent="0.5">
+      <c r="B16" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q16" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="I7" s="3">
+      <c r="R16" s="10">
         <v>0.66666000000000003</v>
       </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.5">
-      <c r="B8" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="3">
-        <v>-0.66666000000000003</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="3">
-        <v>-0.33333000000000002</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8" s="3">
-        <v>0.33333000000000002</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I8" s="3">
+      <c r="S16" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="T16" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="U16" s="11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="17:21" x14ac:dyDescent="0.5">
+      <c r="Q17" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="R17" s="10">
         <v>0.66666000000000003</v>
       </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.5">
-      <c r="B9" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="3">
-        <v>-0.66666000000000003</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" s="3">
-        <v>-0.33333000000000002</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G9" s="3">
-        <v>0</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I9" s="3">
+      <c r="S17" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="T17" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="U17" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="17:21" x14ac:dyDescent="0.5">
+      <c r="Q18" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="R18" s="10">
         <v>0.66666000000000003</v>
       </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.5">
-      <c r="B10" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="3">
-        <v>-1</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="3">
-        <v>-0.33333000000000002</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G10" s="3">
-        <v>0</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I10" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.5">
-      <c r="B11" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="3">
-        <v>-0.66666000000000003</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E11" s="3">
-        <v>-0.33333000000000002</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G11" s="3">
-        <v>0</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="I11" s="3">
-        <v>0.66666000000000003</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.5">
-      <c r="B12" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="3">
-        <v>-1</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E12" s="3">
-        <v>-0.33333000000000002</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G12" s="3">
-        <v>0</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I12" s="3">
-        <v>0.66666000000000003</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.5">
-      <c r="B13" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="3">
-        <v>-0.66666000000000003</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E13" s="3">
-        <v>-0.33333000000000002</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G13" s="3">
-        <v>0.33333000000000002</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="I13" s="3">
-        <v>0.66666000000000003</v>
+      <c r="S18" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="T18" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="U18" s="11" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="B1:R1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>